<commit_message>
adding raw input -ZA
</commit_message>
<xml_diff>
--- a/DowSeq.xlsx
+++ b/DowSeq.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24426"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="2"/>
@@ -877,7 +877,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9375,8 +9375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9916,7 +9916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>139</v>
       </c>
@@ -9946,7 +9946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:13">
       <c r="A18">
         <v>88</v>
       </c>
@@ -9976,7 +9976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>190</v>
       </c>
@@ -10006,7 +10006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:13">
       <c r="A20">
         <v>55</v>
       </c>
@@ -10036,7 +10036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:13">
       <c r="A21">
         <v>171</v>
       </c>
@@ -10066,7 +10066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:13">
       <c r="A22">
         <v>207</v>
       </c>
@@ -10096,7 +10096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:13">
       <c r="A23">
         <v>32</v>
       </c>
@@ -10126,7 +10126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:13">
       <c r="A24">
         <v>5</v>
       </c>
@@ -10156,7 +10156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:13">
       <c r="A25">
         <v>130</v>
       </c>
@@ -10186,7 +10186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:13">
       <c r="A26">
         <v>83</v>
       </c>
@@ -10216,7 +10216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:13">
       <c r="A27">
         <v>185</v>
       </c>
@@ -10246,7 +10246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:13">
       <c r="A28">
         <v>53</v>
       </c>
@@ -10276,7 +10276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:13">
       <c r="A29">
         <v>169</v>
       </c>
@@ -10306,7 +10306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:13">
       <c r="A30">
         <v>205</v>
       </c>
@@ -10335,8 +10335,11 @@
       <c r="I30" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="M30">
+        <v>42.48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31">
         <v>115</v>
       </c>
@@ -10366,7 +10369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:13">
       <c r="A32">
         <v>156</v>
       </c>
@@ -15196,7 +15199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:9">
+    <row r="193" spans="1:13">
       <c r="A193">
         <v>75</v>
       </c>
@@ -15226,7 +15229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:9">
+    <row r="194" spans="1:13">
       <c r="A194">
         <v>68</v>
       </c>
@@ -15256,7 +15259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:9">
+    <row r="195" spans="1:13">
       <c r="A195">
         <v>59</v>
       </c>
@@ -15286,7 +15289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:9">
+    <row r="196" spans="1:13">
       <c r="A196">
         <v>79</v>
       </c>
@@ -15316,7 +15319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:9">
+    <row r="197" spans="1:13">
       <c r="A197">
         <v>51</v>
       </c>
@@ -15346,7 +15349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:9">
+    <row r="198" spans="1:13">
       <c r="A198">
         <v>167</v>
       </c>
@@ -15376,7 +15379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:9">
+    <row r="199" spans="1:13">
       <c r="A199">
         <v>40</v>
       </c>
@@ -15406,7 +15409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:9">
+    <row r="200" spans="1:13">
       <c r="A200">
         <v>23</v>
       </c>
@@ -15436,7 +15439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:9">
+    <row r="201" spans="1:13">
       <c r="A201">
         <v>6</v>
       </c>
@@ -15466,7 +15469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="1:9">
+    <row r="202" spans="1:13">
       <c r="A202">
         <v>44</v>
       </c>
@@ -15496,7 +15499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:9">
+    <row r="203" spans="1:13">
       <c r="A203">
         <v>111</v>
       </c>
@@ -15526,7 +15529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:9">
+    <row r="204" spans="1:13">
       <c r="A204">
         <v>152</v>
       </c>
@@ -15556,7 +15559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:9">
+    <row r="205" spans="1:13">
       <c r="A205">
         <v>11</v>
       </c>
@@ -15586,7 +15589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:9">
+    <row r="206" spans="1:13">
       <c r="A206">
         <v>134</v>
       </c>
@@ -15615,8 +15618,12 @@
       <c r="I206" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="207" spans="1:9">
+      <c r="M206">
+        <f>SUMPRODUCT(M$2:M$5,N$2:N$5)</f>
+        <v>327.21999999999997</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13">
       <c r="A207">
         <v>96</v>
       </c>
@@ -15646,7 +15653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:9">
+    <row r="208" spans="1:13">
       <c r="A208">
         <v>78</v>
       </c>
@@ -15951,7 +15958,7 @@
         <v>15</v>
       </c>
       <c r="B218" s="14">
-        <f t="shared" si="4"/>
+        <f>SUMPRODUCT(C218:I218,R$2:X$2)+SUMPRODUCT(M$2:M$5,N$2:N$5)</f>
         <v>1091.46</v>
       </c>
       <c r="C218" s="3">

</xml_diff>

<commit_message>
added last residue screen -ZA
</commit_message>
<xml_diff>
--- a/DowSeq.xlsx
+++ b/DowSeq.xlsx
@@ -877,7 +877,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9376,7 +9376,7 @@
   <dimension ref="A1:X218"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9467,7 +9467,7 @@
       </c>
       <c r="B2">
         <f>SUMPRODUCT(C2:I2,R$2:X$2)+SUMPRODUCT(M$7:M$10,N$7:N$10)</f>
-        <v>1118.3699999999999</v>
+        <v>730.29</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3">
@@ -9518,7 +9518,7 @@
       </c>
       <c r="B3">
         <f>SUMPRODUCT(C3:I3,R$2:X$2)+SUMPRODUCT(M$7:M$10,N$7:N$10)</f>
-        <v>1135.46</v>
+        <v>747.38</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3">
@@ -9551,7 +9551,7 @@
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B5" si="0">SUMPRODUCT(C4:I4,R$2:X$2)+SUMPRODUCT(M$7:M$10,N$7:N$10)</f>
-        <v>1135.46</v>
+        <v>747.38</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3">
@@ -9584,7 +9584,7 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>1168.45</v>
+        <v>780.37</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3">
@@ -9730,7 +9730,7 @@
         <v>18</v>
       </c>
       <c r="M10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10">
         <v>388.08</v>
@@ -15444,7 +15444,7 @@
         <v>6</v>
       </c>
       <c r="B201" s="14">
-        <f t="shared" ref="B201:B218" si="4">SUMPRODUCT(C201:I201,R$2:X$2)+SUMPRODUCT(M$2:M$5,N$2:N$5)</f>
+        <f t="shared" ref="B201:B217" si="4">SUMPRODUCT(C201:I201,R$2:X$2)+SUMPRODUCT(M$2:M$5,N$2:N$5)</f>
         <v>959.49</v>
       </c>
       <c r="C201" s="3">

</xml_diff>

<commit_message>
implemented permutations function and filter function. Does not yet connect with rest of code but individually, the functions work. - CK
</commit_message>
<xml_diff>
--- a/DowSeq.xlsx
+++ b/DowSeq.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24426"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="2"/>
+    <workbookView xWindow="4240" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sequences" sheetId="3" r:id="rId1"/>
@@ -9376,7 +9376,7 @@
   <dimension ref="A1:X218"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9571,9 +9571,7 @@
       <c r="L4" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="2">
-        <v>0</v>
-      </c>
+      <c r="M4" s="2"/>
       <c r="N4">
         <v>43.02</v>
       </c>

</xml_diff>